<commit_message>
Table and Tableau Updates
</commit_message>
<xml_diff>
--- a/MCU/mcu_box_office.xlsx
+++ b/MCU/mcu_box_office.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\MCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5367C5F7-3477-45A9-9E8E-22F03AECA548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC9923F-598C-44C3-8C12-B7C50AAEE053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mcu_box_office_raw" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,28 @@
     <sheet name="character_theme_box_pivot" sheetId="6" r:id="rId3"/>
     <sheet name="character_theme_rating_pivot" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId5"/>
+    <pivotCache cacheId="21" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>movie_title</t>
   </si>
@@ -257,15 +270,27 @@
   </si>
   <si>
     <t>Average Audience Rating</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -745,7 +770,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -754,16 +779,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -810,13 +832,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="133">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -824,343 +840,7 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1178,22 +858,19 @@
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -1223,9 +900,6 @@
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1240,7 +914,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="codyh" refreshedDate="45336.518506250002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="27">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="codyh" refreshedDate="45336.518506250002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="27" xr:uid="{00000000-000A-0000-FFFF-FFFF14000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
@@ -1751,7 +1425,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Movie Character Theme">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Movie Character Theme">
   <location ref="A1:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -1887,10 +1561,10 @@
     <dataField name="Average Worldwide Box Office" fld="9" subtotal="average" baseField="10" baseItem="2" numFmtId="44"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="129">
+    <format dxfId="13">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1899,7 +1573,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="119">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1909,7 +1583,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="115">
+    <format dxfId="10">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1918,10 +1592,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="9">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -1945,7 +1619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Movie Character Theme">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable5" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Movie Character Theme">
   <location ref="A1:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2078,13 +1752,13 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Total Movies" fld="11" subtotal="count" baseField="10" baseItem="0"/>
-    <dataField name="Average Audience Rating" fld="4" subtotal="average" baseField="10" baseItem="0" numFmtId="171"/>
+    <dataField name="Average Audience Rating" fld="4" subtotal="average" baseField="10" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="14">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2093,7 +1767,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2103,7 +1777,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="4">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2112,7 +1786,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2121,7 +1795,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2130,10 +1804,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="1">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2157,46 +1831,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M28" totalsRowShown="0">
-  <autoFilter ref="A1:M28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:M28" totalsRowShown="0">
+  <autoFilter ref="A1:M28" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="movie_title">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="movie_title">
       <calculatedColumnFormula>mcu_box_office_raw!A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="mcu_phase">
-      <calculatedColumnFormula>mcu_box_office_raw!B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="release_date">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="mcu_phase"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="release_date">
       <calculatedColumnFormula>mcu_box_office_raw!C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="tomato_meter">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="tomato_meter">
       <calculatedColumnFormula>mcu_box_office_raw!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="audience_score">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="audience_score">
       <calculatedColumnFormula>mcu_box_office_raw!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="movie_duration">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="movie_duration">
       <calculatedColumnFormula>mcu_box_office_raw!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="production_budget" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="production_budget" dataCellStyle="Currency">
       <calculatedColumnFormula>mcu_box_office_raw!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="opening_weekend" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="opening_weekend" dataCellStyle="Currency">
       <calculatedColumnFormula>mcu_box_office_raw!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="domestic_box_office" dataCellStyle="Currency">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="domestic_box_office" dataCellStyle="Currency">
       <calculatedColumnFormula>mcu_box_office_raw!I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="worldwide_box_office" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="worldwide_box_office" dataCellStyle="Currency">
       <calculatedColumnFormula>mcu_box_office_raw!J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="character_theme" dataDxfId="132" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="character_theme" dataDxfId="16" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("Spider",A2)),"Spider-Man",IF(ISNUMBER(SEARCH("Doctor",A2)),"Doctor Strange",IF(ISNUMBER(SEARCH("Guardian",A2)),"Guardians of the Galaxy",IF(ISNUMBER(SEARCH("Marvel",A2)),"Captain Marvel",IF(ISNUMBER(SEARCH("Widow",A2)),"Black Widow",IF(ISNUMBER(SEARCH("Shang",A2)),"Shang-Chi",IF(ISNUMBER(SEARCH("Eternals",A2)),"Eternals",IF(ISNUMBER(SEARCH("America",A2)),"Captain America",IF(ISNUMBER(SEARCH("Avengers",A2)),"Avengers",IF(ISNUMBER(SEARCH("Thor",A2)),"Thor",IF(ISNUMBER(SEARCH("Ant",A2)),"Ant-Man",IF(ISNUMBER(SEARCH("Iron",A2)),"Iron Man",IF(ISNUMBER(SEARCH("Hulk",A2)),"Incredible Hulk","")))))))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="character_theme_count" dataDxfId="130" dataCellStyle="Currency">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="character_theme_count" dataDxfId="15" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(K2="Thor",COUNTIF(K:K,"Thor"),IF(K2="Iron Man",COUNTIF(K:K,"Iron Man"),IF(K2="Ant-Man",COUNTIF(K:K,"Ant-Man"),IF(K2="Incredible Hulk",COUNTIF(K:K,"Incredible Hulk"),IF(K2="Captain America",COUNTIF(K:K,"Captain America"),IF(K2="Guardians of the Galaxy",COUNTIF(K:K,"Guardians of the Galaxy"),IF(K2="Avengers",COUNTIF(K:K,"Avengers"),IF(K2="Doctor Strange",COUNTIF(K:K,"Doctor Strange"),IF(K2="Spider-Man",COUNTIF(K:K,"Spider-Man"),IF(K2="Captain Marvel",COUNTIF(K:K,"Captain Marvel"),IF(K2="Black Widow",COUNTIF(K:K,"Black Widow"),IF(K2="Shang-Chi",COUNTIF(K:K,"Shang-Chi"),IF(K2="Eternals",COUNTIF(K:K,"Eternals"),"")))))))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="net_profit" dataDxfId="131" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="net_profit" dataDxfId="14" dataCellStyle="Currency">
       <calculatedColumnFormula>Table2[[#This Row],[worldwide_box_office]]-Table2[[#This Row],[production_budget]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2500,7 +2172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3419,11 +3091,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3489,9 +3161,8 @@
         <f>mcu_box_office_raw!A2</f>
         <v>Iron Man</v>
       </c>
-      <c r="B2">
-        <f>mcu_box_office_raw!B2</f>
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
       <c r="C2" t="str">
         <f>mcu_box_office_raw!C2</f>
@@ -3543,9 +3214,8 @@
         <f>mcu_box_office_raw!A3</f>
         <v>The Incredible Hulk</v>
       </c>
-      <c r="B3">
-        <f>mcu_box_office_raw!B3</f>
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
       <c r="C3" t="str">
         <f>mcu_box_office_raw!C3</f>
@@ -3597,9 +3267,8 @@
         <f>mcu_box_office_raw!A4</f>
         <v>Iron Man 2</v>
       </c>
-      <c r="B4">
-        <f>mcu_box_office_raw!B4</f>
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>77</v>
       </c>
       <c r="C4" t="str">
         <f>mcu_box_office_raw!C4</f>
@@ -3651,9 +3320,8 @@
         <f>mcu_box_office_raw!A5</f>
         <v>Thor</v>
       </c>
-      <c r="B5">
-        <f>mcu_box_office_raw!B5</f>
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>77</v>
       </c>
       <c r="C5" t="str">
         <f>mcu_box_office_raw!C5</f>
@@ -3705,9 +3373,8 @@
         <f>mcu_box_office_raw!A6</f>
         <v>Captain America: The First Avenger</v>
       </c>
-      <c r="B6">
-        <f>mcu_box_office_raw!B6</f>
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>77</v>
       </c>
       <c r="C6" t="str">
         <f>mcu_box_office_raw!C6</f>
@@ -3759,9 +3426,8 @@
         <f>mcu_box_office_raw!A7</f>
         <v>The Avengers</v>
       </c>
-      <c r="B7">
-        <f>mcu_box_office_raw!B7</f>
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>77</v>
       </c>
       <c r="C7" t="str">
         <f>mcu_box_office_raw!C7</f>
@@ -3813,9 +3479,8 @@
         <f>mcu_box_office_raw!A8</f>
         <v>Iron Man 3</v>
       </c>
-      <c r="B8">
-        <f>mcu_box_office_raw!B8</f>
-        <v>2</v>
+      <c r="B8" t="s">
+        <v>78</v>
       </c>
       <c r="C8" t="str">
         <f>mcu_box_office_raw!C8</f>
@@ -3867,9 +3532,8 @@
         <f>mcu_box_office_raw!A9</f>
         <v>Thor: The Dark World</v>
       </c>
-      <c r="B9">
-        <f>mcu_box_office_raw!B9</f>
-        <v>2</v>
+      <c r="B9" t="s">
+        <v>78</v>
       </c>
       <c r="C9" t="str">
         <f>mcu_box_office_raw!C9</f>
@@ -3921,9 +3585,8 @@
         <f>mcu_box_office_raw!A10</f>
         <v>Captain America: The Winter Soldier</v>
       </c>
-      <c r="B10">
-        <f>mcu_box_office_raw!B10</f>
-        <v>2</v>
+      <c r="B10" t="s">
+        <v>78</v>
       </c>
       <c r="C10" t="str">
         <f>mcu_box_office_raw!C10</f>
@@ -3975,9 +3638,8 @@
         <f>mcu_box_office_raw!A11</f>
         <v>Guardians of the Galaxy</v>
       </c>
-      <c r="B11">
-        <f>mcu_box_office_raw!B11</f>
-        <v>2</v>
+      <c r="B11" t="s">
+        <v>78</v>
       </c>
       <c r="C11" t="str">
         <f>mcu_box_office_raw!C11</f>
@@ -4029,9 +3691,8 @@
         <f>mcu_box_office_raw!A12</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="B12">
-        <f>mcu_box_office_raw!B12</f>
-        <v>2</v>
+      <c r="B12" t="s">
+        <v>78</v>
       </c>
       <c r="C12" t="str">
         <f>mcu_box_office_raw!C12</f>
@@ -4083,9 +3744,8 @@
         <f>mcu_box_office_raw!A13</f>
         <v>Ant-Man</v>
       </c>
-      <c r="B13">
-        <f>mcu_box_office_raw!B13</f>
-        <v>2</v>
+      <c r="B13" t="s">
+        <v>78</v>
       </c>
       <c r="C13" t="str">
         <f>mcu_box_office_raw!C13</f>
@@ -4137,9 +3797,8 @@
         <f>mcu_box_office_raw!A14</f>
         <v>Captain America: Civil War</v>
       </c>
-      <c r="B14">
-        <f>mcu_box_office_raw!B14</f>
-        <v>3</v>
+      <c r="B14" t="s">
+        <v>79</v>
       </c>
       <c r="C14" t="str">
         <f>mcu_box_office_raw!C14</f>
@@ -4191,9 +3850,8 @@
         <f>mcu_box_office_raw!A15</f>
         <v>Doctor Strange</v>
       </c>
-      <c r="B15">
-        <f>mcu_box_office_raw!B15</f>
-        <v>3</v>
+      <c r="B15" t="s">
+        <v>79</v>
       </c>
       <c r="C15" t="str">
         <f>mcu_box_office_raw!C15</f>
@@ -4245,9 +3903,8 @@
         <f>mcu_box_office_raw!A16</f>
         <v>Guardians of the Galaxy Vol. 2</v>
       </c>
-      <c r="B16">
-        <f>mcu_box_office_raw!B16</f>
-        <v>3</v>
+      <c r="B16" t="s">
+        <v>79</v>
       </c>
       <c r="C16" t="str">
         <f>mcu_box_office_raw!C16</f>
@@ -4299,9 +3956,8 @@
         <f>mcu_box_office_raw!A17</f>
         <v>Spider-Man: Homecoming</v>
       </c>
-      <c r="B17">
-        <f>mcu_box_office_raw!B17</f>
-        <v>3</v>
+      <c r="B17" t="s">
+        <v>79</v>
       </c>
       <c r="C17" t="str">
         <f>mcu_box_office_raw!C17</f>
@@ -4353,9 +4009,8 @@
         <f>mcu_box_office_raw!A18</f>
         <v>Thor: Ragnarok</v>
       </c>
-      <c r="B18">
-        <f>mcu_box_office_raw!B18</f>
-        <v>3</v>
+      <c r="B18" t="s">
+        <v>79</v>
       </c>
       <c r="C18" t="str">
         <f>mcu_box_office_raw!C18</f>
@@ -4407,9 +4062,8 @@
         <f>mcu_box_office_raw!A19</f>
         <v>Black Panther</v>
       </c>
-      <c r="B19">
-        <f>mcu_box_office_raw!B19</f>
-        <v>3</v>
+      <c r="B19" t="s">
+        <v>79</v>
       </c>
       <c r="C19" t="str">
         <f>mcu_box_office_raw!C19</f>
@@ -4461,9 +4115,8 @@
         <f>mcu_box_office_raw!A20</f>
         <v>Avengers: Infinity War</v>
       </c>
-      <c r="B20">
-        <f>mcu_box_office_raw!B20</f>
-        <v>3</v>
+      <c r="B20" t="s">
+        <v>79</v>
       </c>
       <c r="C20" t="str">
         <f>mcu_box_office_raw!C20</f>
@@ -4515,9 +4168,8 @@
         <f>mcu_box_office_raw!A21</f>
         <v>Ant-Man and the Wasp</v>
       </c>
-      <c r="B21">
-        <f>mcu_box_office_raw!B21</f>
-        <v>3</v>
+      <c r="B21" t="s">
+        <v>79</v>
       </c>
       <c r="C21" t="str">
         <f>mcu_box_office_raw!C21</f>
@@ -4569,9 +4221,8 @@
         <f>mcu_box_office_raw!A22</f>
         <v>Captain Marvel</v>
       </c>
-      <c r="B22">
-        <f>mcu_box_office_raw!B22</f>
-        <v>3</v>
+      <c r="B22" t="s">
+        <v>79</v>
       </c>
       <c r="C22" t="str">
         <f>mcu_box_office_raw!C22</f>
@@ -4623,9 +4274,8 @@
         <f>mcu_box_office_raw!A23</f>
         <v>Avengers: End Game</v>
       </c>
-      <c r="B23">
-        <f>mcu_box_office_raw!B23</f>
-        <v>3</v>
+      <c r="B23" t="s">
+        <v>79</v>
       </c>
       <c r="C23" t="str">
         <f>mcu_box_office_raw!C23</f>
@@ -4677,9 +4327,8 @@
         <f>mcu_box_office_raw!A24</f>
         <v>Spider-Man: Far From Home</v>
       </c>
-      <c r="B24">
-        <f>mcu_box_office_raw!B24</f>
-        <v>3</v>
+      <c r="B24" t="s">
+        <v>79</v>
       </c>
       <c r="C24" t="str">
         <f>mcu_box_office_raw!C24</f>
@@ -4731,9 +4380,8 @@
         <f>mcu_box_office_raw!A25</f>
         <v>Black Widow</v>
       </c>
-      <c r="B25">
-        <f>mcu_box_office_raw!B25</f>
-        <v>4</v>
+      <c r="B25" t="s">
+        <v>80</v>
       </c>
       <c r="C25" t="str">
         <f>mcu_box_office_raw!C25</f>
@@ -4785,9 +4433,8 @@
         <f>mcu_box_office_raw!A26</f>
         <v>Shang-Chi and the Legend of the Ten Rings</v>
       </c>
-      <c r="B26">
-        <f>mcu_box_office_raw!B26</f>
-        <v>4</v>
+      <c r="B26" t="s">
+        <v>80</v>
       </c>
       <c r="C26" t="str">
         <f>mcu_box_office_raw!C26</f>
@@ -4839,9 +4486,8 @@
         <f>mcu_box_office_raw!A27</f>
         <v>Eternals</v>
       </c>
-      <c r="B27">
-        <f>mcu_box_office_raw!B27</f>
-        <v>4</v>
+      <c r="B27" t="s">
+        <v>80</v>
       </c>
       <c r="C27" t="str">
         <f>mcu_box_office_raw!C27</f>
@@ -4893,9 +4539,8 @@
         <f>mcu_box_office_raw!A28</f>
         <v>Spider-Man: No Way Home</v>
       </c>
-      <c r="B28">
-        <f>mcu_box_office_raw!B28</f>
-        <v>4</v>
+      <c r="B28" t="s">
+        <v>80</v>
       </c>
       <c r="C28" t="str">
         <f>mcu_box_office_raw!C28</f>
@@ -4941,6 +4586,9 @@
         <f>Table2[[#This Row],[worldwide_box_office]]-Table2[[#This Row],[production_budget]]</f>
         <v>1691108035</v>
       </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4951,7 +4599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4972,13 +4620,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5142,10 +4790,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -5163,10 +4811,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -5180,7 +4828,7 @@
       <c r="B2" s="6">
         <v>3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>81.666666666666671</v>
       </c>
     </row>
@@ -5191,7 +4839,7 @@
       <c r="B3" s="6">
         <v>4</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>88.75</v>
       </c>
     </row>
@@ -5202,7 +4850,7 @@
       <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>91</v>
       </c>
     </row>
@@ -5213,7 +4861,7 @@
       <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>85.333333333333329</v>
       </c>
     </row>
@@ -5224,7 +4872,7 @@
       <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>45</v>
       </c>
     </row>
@@ -5235,7 +4883,7 @@
       <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>86</v>
       </c>
     </row>
@@ -5246,7 +4894,7 @@
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>78</v>
       </c>
     </row>
@@ -5257,7 +4905,7 @@
       <c r="B9" s="6">
         <v>2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>89.5</v>
       </c>
     </row>
@@ -5268,7 +4916,7 @@
       <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>70</v>
       </c>
     </row>
@@ -5279,7 +4927,7 @@
       <c r="B11" s="6">
         <v>3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>80</v>
       </c>
     </row>
@@ -5290,7 +4938,7 @@
       <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>98</v>
       </c>
     </row>
@@ -5301,7 +4949,7 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>93.333333333333329</v>
       </c>
     </row>
@@ -5312,7 +4960,7 @@
       <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>79.333333333333329</v>
       </c>
     </row>
@@ -5323,7 +4971,7 @@
       <c r="B15" s="6">
         <v>27</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>83.740740740740748</v>
       </c>
     </row>

</xml_diff>